<commit_message>
add item list and error login status has change
</commit_message>
<xml_diff>
--- a/Need.xlsx
+++ b/Need.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1716" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1728" uniqueCount="567">
   <si>
     <t xml:space="preserve">INDO POIPET GROUP</t>
   </si>
@@ -716,16 +716,16 @@
     <t xml:space="preserve">SYSTEM</t>
   </si>
   <si>
-    <t xml:space="preserve">Close cashdraw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start cashdraw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add cash</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Draw cash</t>
+    <t xml:space="preserve">Close Cashdrawer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start Cashdrawer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add Cash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Draw Cash</t>
   </si>
   <si>
     <t xml:space="preserve">C#2022-04-03 13:25:12#2</t>
@@ -3902,7 +3902,7 @@
   <dimension ref="A1:AMJ15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q19" activeCellId="0" sqref="Q19"/>
+      <selection pane="topLeft" activeCell="N19" activeCellId="0" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4013,11 +4013,11 @@
       </c>
       <c r="E3" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087406</v>
+        <v>44710.7062908036</v>
       </c>
       <c r="F3" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087407</v>
+        <v>44710.7062908037</v>
       </c>
       <c r="G3" s="170"/>
       <c r="H3" s="170" t="s">
@@ -4052,14 +4052,14 @@
       </c>
       <c r="T3" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4943523421</v>
+        <v>44710.7060521209</v>
       </c>
       <c r="U3" s="172" t="s">
         <v>201</v>
       </c>
       <c r="V3" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4943523424</v>
+        <v>44710.7060521212</v>
       </c>
       <c r="W3" s="170" t="s">
         <v>202</v>
@@ -4087,11 +4087,11 @@
       </c>
       <c r="E4" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.494408741</v>
+        <v>44710.706290804</v>
       </c>
       <c r="F4" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.494408741</v>
+        <v>44710.706290804</v>
       </c>
       <c r="G4" s="170"/>
       <c r="H4" s="170" t="s">
@@ -4126,16 +4126,18 @@
       </c>
       <c r="T4" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4943523422</v>
+        <v>44710.706052121</v>
       </c>
       <c r="U4" s="172" t="s">
         <v>201</v>
       </c>
       <c r="V4" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4943523424</v>
-      </c>
-      <c r="W4" s="170"/>
+        <v>44710.7060521212</v>
+      </c>
+      <c r="W4" s="170" t="s">
+        <v>202</v>
+      </c>
       <c r="X4" s="170" t="s">
         <v>203</v>
       </c>
@@ -4159,11 +4161,11 @@
       </c>
       <c r="E5" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087413</v>
+        <v>44710.7062908043</v>
       </c>
       <c r="F5" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087413</v>
+        <v>44710.7062908043</v>
       </c>
       <c r="G5" s="170"/>
       <c r="H5" s="170" t="s">
@@ -4198,16 +4200,18 @@
       </c>
       <c r="T5" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4943523422</v>
+        <v>44710.706052121</v>
       </c>
       <c r="U5" s="172" t="s">
         <v>201</v>
       </c>
       <c r="V5" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4943523424</v>
-      </c>
-      <c r="W5" s="170"/>
+        <v>44710.7060521212</v>
+      </c>
+      <c r="W5" s="170" t="s">
+        <v>202</v>
+      </c>
       <c r="X5" s="170" t="s">
         <v>203</v>
       </c>
@@ -4231,11 +4235,11 @@
       </c>
       <c r="E6" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087415</v>
+        <v>44710.7062908045</v>
       </c>
       <c r="F6" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087416</v>
+        <v>44710.7062908046</v>
       </c>
       <c r="G6" s="170"/>
       <c r="H6" s="170" t="s">
@@ -4270,16 +4274,18 @@
       </c>
       <c r="T6" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4943523423</v>
+        <v>44710.706052121</v>
       </c>
       <c r="U6" s="172" t="s">
         <v>201</v>
       </c>
       <c r="V6" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4943523424</v>
-      </c>
-      <c r="W6" s="170"/>
+        <v>44710.7060521212</v>
+      </c>
+      <c r="W6" s="170" t="s">
+        <v>202</v>
+      </c>
       <c r="X6" s="170" t="s">
         <v>203</v>
       </c>
@@ -4303,11 +4309,11 @@
       </c>
       <c r="E7" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087418</v>
+        <v>44710.7062908048</v>
       </c>
       <c r="F7" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087419</v>
+        <v>44710.7062908049</v>
       </c>
       <c r="G7" s="170"/>
       <c r="H7" s="170" t="s">
@@ -4342,16 +4348,18 @@
       </c>
       <c r="T7" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4943523423</v>
+        <v>44710.706052121</v>
       </c>
       <c r="U7" s="172" t="s">
         <v>201</v>
       </c>
       <c r="V7" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4943523424</v>
-      </c>
-      <c r="W7" s="170"/>
+        <v>44710.7060521212</v>
+      </c>
+      <c r="W7" s="170" t="s">
+        <v>202</v>
+      </c>
       <c r="X7" s="170" t="s">
         <v>203</v>
       </c>
@@ -4375,11 +4383,11 @@
       </c>
       <c r="E8" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087421</v>
+        <v>44710.7062908051</v>
       </c>
       <c r="F8" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087421</v>
+        <v>44710.7062908052</v>
       </c>
       <c r="G8" s="170"/>
       <c r="H8" s="170" t="s">
@@ -4414,16 +4422,18 @@
       </c>
       <c r="T8" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4943523423</v>
+        <v>44710.706052121</v>
       </c>
       <c r="U8" s="172" t="s">
         <v>201</v>
       </c>
       <c r="V8" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4943523425</v>
-      </c>
-      <c r="W8" s="170"/>
+        <v>44710.7060521212</v>
+      </c>
+      <c r="W8" s="170" t="s">
+        <v>202</v>
+      </c>
       <c r="X8" s="170" t="s">
         <v>203</v>
       </c>
@@ -4447,11 +4457,11 @@
       </c>
       <c r="E9" s="179" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087424</v>
+        <v>44710.7062908054</v>
       </c>
       <c r="F9" s="179" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087424</v>
+        <v>44710.7062908055</v>
       </c>
       <c r="G9" s="180"/>
       <c r="H9" s="180" t="s">
@@ -4486,16 +4496,18 @@
       </c>
       <c r="T9" s="179" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4943523423</v>
+        <v>44710.7060521211</v>
       </c>
       <c r="U9" s="172" t="s">
         <v>201</v>
       </c>
       <c r="V9" s="179" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4943523425</v>
-      </c>
-      <c r="W9" s="180"/>
+        <v>44710.7060521212</v>
+      </c>
+      <c r="W9" s="170" t="s">
+        <v>202</v>
+      </c>
       <c r="X9" s="180" t="s">
         <v>207</v>
       </c>
@@ -4519,11 +4531,11 @@
       </c>
       <c r="E10" s="179" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087426</v>
+        <v>44710.7062908057</v>
       </c>
       <c r="F10" s="179" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087427</v>
+        <v>44710.7062908057</v>
       </c>
       <c r="G10" s="180"/>
       <c r="H10" s="180" t="s">
@@ -4558,16 +4570,18 @@
       </c>
       <c r="T10" s="179" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4943523423</v>
+        <v>44710.7060521211</v>
       </c>
       <c r="U10" s="172" t="s">
         <v>201</v>
       </c>
       <c r="V10" s="179" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4943523425</v>
-      </c>
-      <c r="W10" s="180"/>
+        <v>44710.7060521212</v>
+      </c>
+      <c r="W10" s="170" t="s">
+        <v>202</v>
+      </c>
       <c r="X10" s="180" t="s">
         <v>207</v>
       </c>
@@ -4591,11 +4605,11 @@
       </c>
       <c r="E11" s="179" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087429</v>
+        <v>44710.706290806</v>
       </c>
       <c r="F11" s="179" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.494408743</v>
+        <v>44710.706290806</v>
       </c>
       <c r="G11" s="180"/>
       <c r="H11" s="180" t="s">
@@ -4630,16 +4644,18 @@
       </c>
       <c r="T11" s="179" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4943523423</v>
+        <v>44710.7060521211</v>
       </c>
       <c r="U11" s="172" t="s">
         <v>201</v>
       </c>
       <c r="V11" s="179" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4943523425</v>
-      </c>
-      <c r="W11" s="180"/>
+        <v>44710.7060521213</v>
+      </c>
+      <c r="W11" s="170" t="s">
+        <v>202</v>
+      </c>
       <c r="X11" s="180" t="s">
         <v>207</v>
       </c>
@@ -4663,11 +4679,11 @@
       </c>
       <c r="E12" s="179" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087432</v>
+        <v>44710.7062908062</v>
       </c>
       <c r="F12" s="179" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087433</v>
+        <v>44710.7062908063</v>
       </c>
       <c r="G12" s="180"/>
       <c r="H12" s="180" t="s">
@@ -4702,16 +4718,18 @@
       </c>
       <c r="T12" s="179" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4943523423</v>
+        <v>44710.7060521211</v>
       </c>
       <c r="U12" s="172" t="s">
         <v>201</v>
       </c>
       <c r="V12" s="179" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4943523425</v>
-      </c>
-      <c r="W12" s="180"/>
+        <v>44710.7060521213</v>
+      </c>
+      <c r="W12" s="170" t="s">
+        <v>202</v>
+      </c>
       <c r="X12" s="180" t="s">
         <v>207</v>
       </c>
@@ -4735,11 +4753,11 @@
       </c>
       <c r="E13" s="179" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087435</v>
+        <v>44710.7062908065</v>
       </c>
       <c r="F13" s="179" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087435</v>
+        <v>44710.7062908066</v>
       </c>
       <c r="G13" s="180"/>
       <c r="H13" s="180" t="s">
@@ -4774,16 +4792,18 @@
       </c>
       <c r="T13" s="179" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4943523423</v>
+        <v>44710.7060521211</v>
       </c>
       <c r="U13" s="172" t="s">
         <v>201</v>
       </c>
       <c r="V13" s="179" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4943523425</v>
-      </c>
-      <c r="W13" s="180"/>
+        <v>44710.7060521213</v>
+      </c>
+      <c r="W13" s="170" t="s">
+        <v>202</v>
+      </c>
       <c r="X13" s="180" t="s">
         <v>207</v>
       </c>
@@ -4807,11 +4827,11 @@
       </c>
       <c r="E14" s="179" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087438</v>
+        <v>44710.7062908068</v>
       </c>
       <c r="F14" s="179" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087438</v>
+        <v>44710.7062908069</v>
       </c>
       <c r="G14" s="180"/>
       <c r="H14" s="180" t="s">
@@ -4846,16 +4866,18 @@
       </c>
       <c r="T14" s="179" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4943523424</v>
+        <v>44710.7060521211</v>
       </c>
       <c r="U14" s="172" t="s">
         <v>201</v>
       </c>
       <c r="V14" s="179" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4943523425</v>
-      </c>
-      <c r="W14" s="180"/>
+        <v>44710.7060521213</v>
+      </c>
+      <c r="W14" s="170" t="s">
+        <v>202</v>
+      </c>
       <c r="X14" s="180" t="s">
         <v>207</v>
       </c>
@@ -4879,11 +4901,11 @@
       </c>
       <c r="E15" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.494408744</v>
+        <v>44710.7062908071</v>
       </c>
       <c r="F15" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087441</v>
+        <v>44710.7062908071</v>
       </c>
       <c r="G15" s="170"/>
       <c r="H15" s="170" t="s">
@@ -4918,16 +4940,18 @@
       </c>
       <c r="T15" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4943523424</v>
+        <v>44710.7060521211</v>
       </c>
       <c r="U15" s="172" t="s">
         <v>201</v>
       </c>
       <c r="V15" s="173" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4943523425</v>
-      </c>
-      <c r="W15" s="170"/>
+        <v>44710.7060521213</v>
+      </c>
+      <c r="W15" s="170" t="s">
+        <v>202</v>
+      </c>
       <c r="X15" s="170" t="s">
         <v>203</v>
       </c>
@@ -5029,11 +5053,11 @@
       </c>
       <c r="E3" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087759</v>
+        <v>44710.7062908407</v>
       </c>
       <c r="F3" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.494408776</v>
+        <v>44710.7062908408</v>
       </c>
       <c r="G3" s="181"/>
       <c r="H3" s="181" t="s">
@@ -5041,7 +5065,7 @@
       </c>
       <c r="I3" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.4944087761#1</v>
+        <v>c#44710.7062908409#1</v>
       </c>
     </row>
     <row r="4" s="159" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5059,11 +5083,11 @@
       </c>
       <c r="E4" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087765</v>
+        <v>44710.7062908413</v>
       </c>
       <c r="F4" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087766</v>
+        <v>44710.7062908414</v>
       </c>
       <c r="G4" s="181"/>
       <c r="H4" s="181" t="s">
@@ -5071,7 +5095,7 @@
       </c>
       <c r="I4" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.4944087766#1</v>
+        <v>c#44710.7062908415#1</v>
       </c>
     </row>
     <row r="5" s="159" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5089,11 +5113,11 @@
       </c>
       <c r="E5" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087768</v>
+        <v>44710.7062908417</v>
       </c>
       <c r="F5" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087769</v>
+        <v>44710.7062908417</v>
       </c>
       <c r="G5" s="181"/>
       <c r="H5" s="181" t="s">
@@ -5101,7 +5125,7 @@
       </c>
       <c r="I5" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.4944087769#1</v>
+        <v>c#44710.7062908418#1</v>
       </c>
     </row>
     <row r="6" s="159" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5119,11 +5143,11 @@
       </c>
       <c r="E6" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087771</v>
+        <v>44710.706290842</v>
       </c>
       <c r="F6" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087772</v>
+        <v>44710.706290842</v>
       </c>
       <c r="G6" s="181"/>
       <c r="H6" s="181" t="s">
@@ -5131,7 +5155,7 @@
       </c>
       <c r="I6" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.4944087772#1</v>
+        <v>c#44710.7062908421#1</v>
       </c>
     </row>
     <row r="7" s="159" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5149,11 +5173,11 @@
       </c>
       <c r="E7" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087774</v>
+        <v>44710.7062908423</v>
       </c>
       <c r="F7" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087775</v>
+        <v>44710.7062908424</v>
       </c>
       <c r="G7" s="181"/>
       <c r="H7" s="181" t="s">
@@ -5161,7 +5185,7 @@
       </c>
       <c r="I7" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.4944087775#1</v>
+        <v>c#44710.7062908424#1</v>
       </c>
     </row>
     <row r="8" s="159" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5179,11 +5203,11 @@
       </c>
       <c r="E8" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087777</v>
+        <v>44710.7062908426</v>
       </c>
       <c r="F8" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087778</v>
+        <v>44710.7062908427</v>
       </c>
       <c r="G8" s="181"/>
       <c r="H8" s="181" t="s">
@@ -5191,7 +5215,7 @@
       </c>
       <c r="I8" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.4944087779#1</v>
+        <v>c#44710.7062908427#1</v>
       </c>
     </row>
     <row r="9" s="159" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5209,11 +5233,11 @@
       </c>
       <c r="E9" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087781</v>
+        <v>44710.7062908429</v>
       </c>
       <c r="F9" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087781</v>
+        <v>44710.706290843</v>
       </c>
       <c r="G9" s="181"/>
       <c r="H9" s="181" t="s">
@@ -5221,7 +5245,7 @@
       </c>
       <c r="I9" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.4944087782#1</v>
+        <v>c#44710.7062908431#1</v>
       </c>
     </row>
     <row r="10" s="159" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5239,11 +5263,11 @@
       </c>
       <c r="E10" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087784</v>
+        <v>44710.7062908432</v>
       </c>
       <c r="F10" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087784</v>
+        <v>44710.7062908433</v>
       </c>
       <c r="G10" s="181"/>
       <c r="H10" s="181" t="s">
@@ -5251,7 +5275,7 @@
       </c>
       <c r="I10" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.4944087785#1</v>
+        <v>c#44710.7062908434#1</v>
       </c>
     </row>
     <row r="11" s="159" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5269,11 +5293,11 @@
       </c>
       <c r="E11" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087787</v>
+        <v>44710.7062908436</v>
       </c>
       <c r="F11" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087788</v>
+        <v>44710.7062908436</v>
       </c>
       <c r="G11" s="181"/>
       <c r="H11" s="181" t="s">
@@ -5281,7 +5305,7 @@
       </c>
       <c r="I11" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.4944087788#1</v>
+        <v>c#44710.7062908437#1</v>
       </c>
     </row>
     <row r="12" s="159" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5299,11 +5323,11 @@
       </c>
       <c r="E12" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087791</v>
+        <v>44710.7062908439</v>
       </c>
       <c r="F12" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087791</v>
+        <v>44710.7062908439</v>
       </c>
       <c r="G12" s="181"/>
       <c r="H12" s="181" t="s">
@@ -5311,7 +5335,7 @@
       </c>
       <c r="I12" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.4944087792#1</v>
+        <v>c#44710.706290844#1</v>
       </c>
     </row>
     <row r="13" s="159" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5329,11 +5353,11 @@
       </c>
       <c r="E13" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087794</v>
+        <v>44710.7062908442</v>
       </c>
       <c r="F13" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087794</v>
+        <v>44710.7062908443</v>
       </c>
       <c r="G13" s="181"/>
       <c r="H13" s="181" t="s">
@@ -5341,7 +5365,7 @@
       </c>
       <c r="I13" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.4944087795#1</v>
+        <v>c#44710.7062908443#1</v>
       </c>
     </row>
     <row r="14" s="159" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5359,11 +5383,11 @@
       </c>
       <c r="E14" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087797</v>
+        <v>44710.7062908445</v>
       </c>
       <c r="F14" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087798</v>
+        <v>44710.7062908446</v>
       </c>
       <c r="G14" s="181"/>
       <c r="H14" s="181" t="s">
@@ -5371,7 +5395,7 @@
       </c>
       <c r="I14" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.4944087798#1</v>
+        <v>c#44710.7062908447#1</v>
       </c>
     </row>
     <row r="15" s="159" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5389,11 +5413,11 @@
       </c>
       <c r="E15" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.49440878</v>
+        <v>44710.7062908448</v>
       </c>
       <c r="F15" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087801</v>
+        <v>44710.7062908449</v>
       </c>
       <c r="G15" s="181"/>
       <c r="H15" s="181" t="s">
@@ -5401,7 +5425,7 @@
       </c>
       <c r="I15" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.4944087802#1</v>
+        <v>c#44710.706290845#1</v>
       </c>
     </row>
     <row r="16" s="159" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5419,11 +5443,11 @@
       </c>
       <c r="E16" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087804</v>
+        <v>44710.7062908451</v>
       </c>
       <c r="F16" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087804</v>
+        <v>44710.7062908452</v>
       </c>
       <c r="G16" s="181"/>
       <c r="H16" s="181" t="s">
@@ -5431,7 +5455,7 @@
       </c>
       <c r="I16" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.4944087805#1</v>
+        <v>c#44710.7062908453#1</v>
       </c>
     </row>
     <row r="17" s="159" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5449,11 +5473,11 @@
       </c>
       <c r="E17" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087807</v>
+        <v>44710.7062908455</v>
       </c>
       <c r="F17" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087807</v>
+        <v>44710.7062908455</v>
       </c>
       <c r="G17" s="181"/>
       <c r="H17" s="181" t="s">
@@ -5461,7 +5485,7 @@
       </c>
       <c r="I17" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.4944087808#1</v>
+        <v>c#44710.7062908456#1</v>
       </c>
     </row>
     <row r="18" s="159" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5479,11 +5503,11 @@
       </c>
       <c r="E18" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.494408781</v>
+        <v>44710.7062908458</v>
       </c>
       <c r="F18" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.494408781</v>
+        <v>44710.7062908458</v>
       </c>
       <c r="G18" s="181"/>
       <c r="H18" s="181" t="s">
@@ -5491,7 +5515,7 @@
       </c>
       <c r="I18" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.4944087811#1</v>
+        <v>c#44710.7062908459#1</v>
       </c>
     </row>
     <row r="19" s="159" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5509,11 +5533,11 @@
       </c>
       <c r="E19" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087813</v>
+        <v>44710.7062908461</v>
       </c>
       <c r="F19" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087814</v>
+        <v>44710.7062908462</v>
       </c>
       <c r="G19" s="181"/>
       <c r="H19" s="181" t="s">
@@ -5521,7 +5545,7 @@
       </c>
       <c r="I19" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.4944087815#1</v>
+        <v>c#44710.7062908462#1</v>
       </c>
     </row>
     <row r="20" s="159" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5539,11 +5563,11 @@
       </c>
       <c r="E20" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087816</v>
+        <v>44710.7062908464</v>
       </c>
       <c r="F20" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087817</v>
+        <v>44710.7062908465</v>
       </c>
       <c r="G20" s="181"/>
       <c r="H20" s="181" t="s">
@@ -5551,7 +5575,7 @@
       </c>
       <c r="I20" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.4944087818#1</v>
+        <v>c#44710.7062908466#1</v>
       </c>
     </row>
     <row r="21" s="159" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5569,11 +5593,11 @@
       </c>
       <c r="E21" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087819</v>
+        <v>44710.7062908467</v>
       </c>
       <c r="F21" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.494408782</v>
+        <v>44710.7062908468</v>
       </c>
       <c r="G21" s="181"/>
       <c r="H21" s="181" t="s">
@@ -5581,7 +5605,7 @@
       </c>
       <c r="I21" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.4944087821#1</v>
+        <v>c#44710.7062908469#1</v>
       </c>
     </row>
     <row r="22" s="159" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5599,11 +5623,11 @@
       </c>
       <c r="E22" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087823</v>
+        <v>44710.706290847</v>
       </c>
       <c r="F22" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087823</v>
+        <v>44710.7062908471</v>
       </c>
       <c r="G22" s="181"/>
       <c r="H22" s="181" t="s">
@@ -5611,7 +5635,7 @@
       </c>
       <c r="I22" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.4944087824#1</v>
+        <v>c#44710.7062908472#1</v>
       </c>
     </row>
     <row r="23" s="159" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5629,11 +5653,11 @@
       </c>
       <c r="E23" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087826</v>
+        <v>44710.7062908474</v>
       </c>
       <c r="F23" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087826</v>
+        <v>44710.7062908474</v>
       </c>
       <c r="G23" s="181"/>
       <c r="H23" s="181" t="s">
@@ -5641,7 +5665,7 @@
       </c>
       <c r="I23" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.4944087827#1</v>
+        <v>c#44710.7062908475#1</v>
       </c>
     </row>
     <row r="24" s="159" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5659,11 +5683,11 @@
       </c>
       <c r="E24" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087829</v>
+        <v>44710.7062908477</v>
       </c>
       <c r="F24" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.494408783</v>
+        <v>44710.7062908477</v>
       </c>
       <c r="G24" s="181"/>
       <c r="H24" s="181" t="s">
@@ -5671,7 +5695,7 @@
       </c>
       <c r="I24" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.494408783#1</v>
+        <v>c#44710.7062908478#1</v>
       </c>
     </row>
     <row r="25" s="159" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5689,11 +5713,11 @@
       </c>
       <c r="E25" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087832</v>
+        <v>44710.706290848</v>
       </c>
       <c r="F25" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087833</v>
+        <v>44710.7062908481</v>
       </c>
       <c r="G25" s="181"/>
       <c r="H25" s="181" t="s">
@@ -5701,7 +5725,7 @@
       </c>
       <c r="I25" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.4944087834#1</v>
+        <v>c#44710.7062908481#1</v>
       </c>
     </row>
     <row r="26" s="159" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5719,11 +5743,11 @@
       </c>
       <c r="E26" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087835</v>
+        <v>44710.7062908483</v>
       </c>
       <c r="F26" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087836</v>
+        <v>44710.7062908484</v>
       </c>
       <c r="G26" s="181"/>
       <c r="H26" s="181" t="s">
@@ -5731,7 +5755,7 @@
       </c>
       <c r="I26" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.4944087837#1</v>
+        <v>c#44710.7062908485#1</v>
       </c>
     </row>
     <row r="27" s="159" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5749,11 +5773,11 @@
       </c>
       <c r="E27" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087839</v>
+        <v>44710.7062908486</v>
       </c>
       <c r="F27" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944087839</v>
+        <v>44710.7062908487</v>
       </c>
       <c r="G27" s="181"/>
       <c r="H27" s="181" t="s">
@@ -5761,7 +5785,7 @@
       </c>
       <c r="I27" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.494408784#1</v>
+        <v>c#44710.7062908488#1</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5887,11 +5911,11 @@
       </c>
       <c r="G3" s="186" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944088166</v>
+        <v>44710.7062909014</v>
       </c>
       <c r="H3" s="186" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944088167</v>
+        <v>44710.7062909016</v>
       </c>
       <c r="I3" s="184"/>
       <c r="J3" s="184" t="s">
@@ -5899,7 +5923,7 @@
       </c>
       <c r="K3" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.4944088168#1</v>
+        <v>c#44710.7062909017#1</v>
       </c>
       <c r="L3" s="181" t="n">
         <v>0</v>
@@ -5926,11 +5950,11 @@
       </c>
       <c r="G4" s="186" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944088171</v>
+        <v>44710.706290902</v>
       </c>
       <c r="H4" s="186" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944088171</v>
+        <v>44710.7062909021</v>
       </c>
       <c r="I4" s="184"/>
       <c r="J4" s="184" t="s">
@@ -5938,7 +5962,7 @@
       </c>
       <c r="K4" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.4944088172#1</v>
+        <v>c#44710.7062909022#1</v>
       </c>
       <c r="L4" s="181" t="n">
         <v>1</v>
@@ -5965,11 +5989,11 @@
       </c>
       <c r="G5" s="186" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944088174</v>
+        <v>44710.7062909024</v>
       </c>
       <c r="H5" s="186" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944088175</v>
+        <v>44710.7062909025</v>
       </c>
       <c r="I5" s="184"/>
       <c r="J5" s="184" t="s">
@@ -5977,7 +6001,7 @@
       </c>
       <c r="K5" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.4944088176#1</v>
+        <v>c#44710.7062909025#1</v>
       </c>
       <c r="L5" s="181" t="n">
         <v>2</v>
@@ -7359,11 +7383,11 @@
       </c>
       <c r="F3" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944089003</v>
+        <v>44710.7062909926</v>
       </c>
       <c r="G3" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944089005</v>
+        <v>44710.7062909928</v>
       </c>
       <c r="H3" s="181"/>
       <c r="I3" s="181" t="s">
@@ -7371,7 +7395,7 @@
       </c>
       <c r="J3" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.4944089006#1</v>
+        <v>c#44710.7062909928#1</v>
       </c>
     </row>
     <row r="4" s="159" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7392,11 +7416,11 @@
       </c>
       <c r="F4" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944089009</v>
+        <v>44710.7062909931</v>
       </c>
       <c r="G4" s="183" t="n">
         <f aca="true">NOW()</f>
-        <v>44709.4944089009</v>
+        <v>44710.7062909932</v>
       </c>
       <c r="H4" s="181"/>
       <c r="I4" s="181" t="s">
@@ -7404,7 +7428,7 @@
       </c>
       <c r="J4" s="181" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44709.494408901#1</v>
+        <v>c#44710.7062909933#1</v>
       </c>
     </row>
   </sheetData>
@@ -16169,7 +16193,7 @@
       </c>
       <c r="B4" s="128" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16230,7 +16254,7 @@
       </c>
       <c r="B11" s="128" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16239,7 +16263,7 @@
       </c>
       <c r="B12" s="128" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16387,7 +16411,7 @@
       </c>
       <c r="B4" s="137" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="C4" s="127" t="n">
         <v>1</v>
@@ -16414,11 +16438,11 @@
       </c>
       <c r="L4" s="141" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="M4" s="141" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="N4" s="129" t="n">
         <v>3</v>
@@ -16437,7 +16461,7 @@
       </c>
       <c r="B5" s="137" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="C5" s="129" t="s">
         <v>146</v>
@@ -16464,11 +16488,11 @@
       </c>
       <c r="L5" s="141" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="M5" s="141" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="N5" s="129" t="n">
         <v>3</v>
@@ -16487,7 +16511,7 @@
       </c>
       <c r="B6" s="137" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="C6" s="129" t="s">
         <v>146</v>
@@ -16514,11 +16538,11 @@
       </c>
       <c r="L6" s="141" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="M6" s="141" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="N6" s="129" t="n">
         <v>3</v>
@@ -16537,7 +16561,7 @@
       </c>
       <c r="B7" s="137" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="C7" s="129" t="s">
         <v>146</v>
@@ -16564,11 +16588,11 @@
       </c>
       <c r="L7" s="141" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="M7" s="141" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="N7" s="129" t="n">
         <v>3</v>
@@ -16587,7 +16611,7 @@
       </c>
       <c r="B8" s="137" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="C8" s="127" t="n">
         <v>1</v>
@@ -16615,11 +16639,11 @@
       </c>
       <c r="L8" s="141" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="M8" s="141" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="N8" s="129" t="n">
         <v>3</v>
@@ -16638,7 +16662,7 @@
       </c>
       <c r="B9" s="137" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="C9" s="127" t="n">
         <v>1</v>
@@ -16666,11 +16690,11 @@
       </c>
       <c r="L9" s="141" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="M9" s="141" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="N9" s="129" t="n">
         <v>3</v>
@@ -16689,7 +16713,7 @@
       </c>
       <c r="B10" s="137" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="C10" s="127" t="n">
         <v>1</v>
@@ -16730,7 +16754,7 @@
       </c>
       <c r="B11" s="137" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="C11" s="127" t="n">
         <v>1</v>
@@ -16771,7 +16795,7 @@
       </c>
       <c r="B12" s="137" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="C12" s="127" t="n">
         <v>2</v>
@@ -16812,7 +16836,7 @@
       </c>
       <c r="B13" s="137" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="C13" s="127" t="n">
         <v>2</v>
@@ -16853,7 +16877,7 @@
       </c>
       <c r="B14" s="137" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="C14" s="127" t="n">
         <v>2</v>
@@ -16894,7 +16918,7 @@
       </c>
       <c r="B15" s="137" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="C15" s="127" t="n">
         <v>2</v>
@@ -16935,7 +16959,7 @@
       </c>
       <c r="B16" s="137" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="C16" s="127" t="n">
         <v>2</v>
@@ -16976,7 +17000,7 @@
       </c>
       <c r="B17" s="137" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="C17" s="127" t="n">
         <v>2</v>
@@ -17256,11 +17280,11 @@
       <c r="G3" s="163"/>
       <c r="H3" s="167" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="I3" s="167" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="J3" s="163" t="s">
         <v>182</v>
@@ -17291,11 +17315,11 @@
       <c r="G4" s="163"/>
       <c r="H4" s="167" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="I4" s="167" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="J4" s="163" t="s">
         <v>182</v>
@@ -17326,11 +17350,11 @@
       <c r="G5" s="163"/>
       <c r="H5" s="167" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="I5" s="167" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="J5" s="163" t="s">
         <v>188</v>
@@ -17361,11 +17385,11 @@
       <c r="G6" s="163"/>
       <c r="H6" s="167" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="I6" s="167" t="n">
         <f aca="true">TODAY()</f>
-        <v>44709</v>
+        <v>44710</v>
       </c>
       <c r="J6" s="163" t="s">
         <v>188</v>

</xml_diff>

<commit_message>
modify cash transaction on use on field
</commit_message>
<xml_diff>
--- a/Need.xlsx
+++ b/Need.xlsx
@@ -242,7 +242,6 @@
         <color rgb="FF000000"/>
         <rFont val="Kalinga"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Working Permith </t>
     </r>
@@ -661,7 +660,6 @@
         <color rgb="FF2A6099"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">to</t>
     </r>
@@ -672,7 +670,6 @@
         <color rgb="FF2A6099"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> dolla rate#35.33</t>
     </r>
@@ -684,7 +681,6 @@
         <color rgb="FF2A6099"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">from </t>
     </r>
@@ -695,7 +691,6 @@
         <color rgb="FF2A6099"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">bath rate#35.33</t>
     </r>
@@ -899,7 +894,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">បង្កើតអ្នកប្រើជា </t>
     </r>
@@ -909,7 +903,6 @@
         <color rgb="FF000000"/>
         <rFont val="Khmer OS"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Admin</t>
     </r>
@@ -921,7 +914,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">បើមិនមានអ្នកប្រើ ត្រូវចុះឈ្មោះអ្នកប្រើជា</t>
     </r>
@@ -931,7 +923,6 @@
         <color rgb="FF000000"/>
         <rFont val="Khmer OS"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Admin</t>
     </r>
@@ -941,7 +932,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ជាមុន</t>
     </r>
@@ -956,7 +946,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">អ្នកប្រើ </t>
     </r>
@@ -966,7 +955,6 @@
         <color rgb="FF000000"/>
         <rFont val="Khmer OS"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Log in</t>
     </r>
@@ -978,7 +966,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ទំព័រ </t>
     </r>
@@ -988,7 +975,6 @@
         <color rgb="FF000000"/>
         <rFont val="Khmer OS"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Dashboard</t>
     </r>
@@ -1039,7 +1025,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ប្រភេទលុយ</t>
     </r>
@@ -1049,7 +1034,6 @@
         <color rgb="FF000000"/>
         <rFont val="Khmer OS"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -1059,7 +1043,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">រូបិយប័ណ្ណ</t>
     </r>
@@ -1069,7 +1052,6 @@
         <color rgb="FF000000"/>
         <rFont val="Khmer OS"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -2067,7 +2049,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2090,7 +2071,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2098,7 +2078,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -2110,21 +2089,18 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="14"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2132,7 +2108,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2140,7 +2115,6 @@
       <color rgb="FFFFFF00"/>
       <name val="Aharoni"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2148,7 +2122,6 @@
       <color rgb="FFFFFF00"/>
       <name val="Aharoni"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2156,14 +2129,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2171,7 +2142,6 @@
       <color rgb="FF000000"/>
       <name val="Kalinga"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2179,7 +2149,6 @@
       <color rgb="FF000000"/>
       <name val="Kalinga"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2195,21 +2164,18 @@
       <color rgb="FFFF0000"/>
       <name val="Kalinga"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Kalinga"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Kalinga"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2218,21 +2184,18 @@
       <color rgb="FF000000"/>
       <name val="Kalinga"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2240,42 +2203,36 @@
       <color rgb="FFEEEEEE"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFEEEEEE"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFC9211E"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF861141"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="16"/>
       <color rgb="FF468A1A"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF2A6099"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2283,14 +2240,12 @@
       <color rgb="FF2A6099"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF468A1A"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2298,28 +2253,24 @@
       <color rgb="FF468A1A"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF127622"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF7B3D00"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Khmer OS"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="50">
@@ -2343,8 +2294,8 @@
     </fill>
     <fill>
       <patternFill patternType="darkGray">
-        <fgColor rgb="FF045F10"/>
-        <bgColor rgb="FF157345"/>
+        <fgColor rgb="FF05630F"/>
+        <bgColor rgb="FF146F3D"/>
       </patternFill>
     </fill>
     <fill>
@@ -2355,7 +2306,7 @@
     </fill>
     <fill>
       <patternFill patternType="darkGray">
-        <fgColor rgb="FF0896D5"/>
+        <fgColor rgb="FF089BCB"/>
         <bgColor rgb="FF00FFFF"/>
       </patternFill>
     </fill>
@@ -2392,7 +2343,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00FFFF"/>
-        <bgColor rgb="FF0896D5"/>
+        <bgColor rgb="FF089BCB"/>
       </patternFill>
     </fill>
     <fill>
@@ -2403,8 +2354,8 @@
     </fill>
     <fill>
       <patternFill patternType="mediumGray">
-        <fgColor rgb="FF157345"/>
-        <bgColor rgb="FF0896D5"/>
+        <fgColor rgb="FF089BCB"/>
+        <bgColor rgb="FF146F3D"/>
       </patternFill>
     </fill>
     <fill>
@@ -2421,7 +2372,7 @@
     </fill>
     <fill>
       <patternFill patternType="darkGray">
-        <fgColor rgb="FF157345"/>
+        <fgColor rgb="FF146F3D"/>
         <bgColor rgb="FF468A1A"/>
       </patternFill>
     </fill>
@@ -2547,7 +2498,7 @@
     </fill>
     <fill>
       <patternFill patternType="darkGray">
-        <fgColor rgb="FF8E0715"/>
+        <fgColor rgb="FF8F0710"/>
         <bgColor rgb="FF8D281E"/>
       </patternFill>
     </fill>
@@ -2565,14 +2516,14 @@
     </fill>
     <fill>
       <patternFill patternType="darkGray">
-        <fgColor rgb="FF157345"/>
-        <bgColor rgb="FF045F10"/>
+        <fgColor rgb="FF146F3D"/>
+        <bgColor rgb="FF05630F"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF28471F"/>
-        <bgColor rgb="FF045F10"/>
+        <bgColor rgb="FF05630F"/>
       </patternFill>
     </fill>
     <fill>
@@ -3921,7 +3872,6 @@
     <dxf>
       <font>
         <name val="Calibri"/>
-        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF000000"/>
         <sz val="11"/>
@@ -3935,7 +3885,6 @@
     <dxf>
       <font>
         <name val="Calibri"/>
-        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF9C6500"/>
         <sz val="11"/>
@@ -3949,7 +3898,6 @@
     <dxf>
       <font>
         <name val="Calibri"/>
-        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF006100"/>
         <sz val="11"/>
@@ -3963,7 +3911,6 @@
     <dxf>
       <font>
         <name val="Calibri"/>
-        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF000000"/>
         <sz val="11"/>
@@ -3977,7 +3924,6 @@
     <dxf>
       <font>
         <name val="Calibri"/>
-        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF9C6500"/>
         <sz val="11"/>
@@ -3991,7 +3937,6 @@
     <dxf>
       <font>
         <name val="Calibri"/>
-        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF006100"/>
         <sz val="11"/>
@@ -4005,7 +3950,6 @@
     <dxf>
       <font>
         <name val="Calibri"/>
-        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF9C0006"/>
         <sz val="11"/>
@@ -4019,7 +3963,6 @@
     <dxf>
       <font>
         <name val="Calibri"/>
-        <charset val="1"/>
         <family val="2"/>
         <b val="1"/>
         <i val="0"/>
@@ -4030,7 +3973,6 @@
     <dxf>
       <font>
         <name val="Calibri"/>
-        <charset val="1"/>
         <family val="2"/>
         <b val="1"/>
         <i val="0"/>
@@ -4050,12 +3992,12 @@
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF3300"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF8E0715"/>
-      <rgbColor rgb="FF045F10"/>
+      <rgbColor rgb="FF8F0710"/>
+      <rgbColor rgb="FF05630F"/>
       <rgbColor rgb="FFFFE699"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF67105C"/>
-      <rgbColor rgb="FF157345"/>
+      <rgbColor rgb="FF146F3D"/>
       <rgbColor rgb="FFBFBFBF"/>
       <rgbColor rgb="FF706E0C"/>
       <rgbColor rgb="FF8FAADC"/>
@@ -4072,7 +4014,7 @@
       <rgbColor rgb="FFC5E0B4"/>
       <rgbColor rgb="FFBF0041"/>
       <rgbColor rgb="FF58112A"/>
-      <rgbColor rgb="FF0896D5"/>
+      <rgbColor rgb="FF089BCB"/>
       <rgbColor rgb="FFEEEEEE"/>
       <rgbColor rgb="FFAFD095"/>
       <rgbColor rgb="FFE2F0D9"/>
@@ -4114,9 +4056,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>654840</xdr:colOff>
+      <xdr:colOff>654480</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>100440</xdr:rowOff>
+      <xdr:rowOff>100080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4126,7 +4068,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="101520" y="56880"/>
-          <a:ext cx="3994920" cy="1270440"/>
+          <a:ext cx="3996720" cy="1270080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4259,9 +4201,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>260640</xdr:colOff>
+      <xdr:colOff>260280</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>154440</xdr:rowOff>
+      <xdr:rowOff>154080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4271,7 +4213,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="41760" y="1639080"/>
-          <a:ext cx="5289840" cy="2546280"/>
+          <a:ext cx="5292720" cy="2545920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4550,9 +4492,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>187920</xdr:colOff>
+      <xdr:colOff>187560</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:rowOff>153720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4562,7 +4504,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="88200" y="4299120"/>
-          <a:ext cx="5170680" cy="2339640"/>
+          <a:ext cx="5173560" cy="2339280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4750,7 +4692,7 @@
       <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.22"/>
   </cols>
@@ -4863,11 +4805,11 @@
       <c r="G3" s="190"/>
       <c r="H3" s="194" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="I3" s="194" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="J3" s="190" t="s">
         <v>223</v>
@@ -4895,11 +4837,11 @@
       <c r="G4" s="190"/>
       <c r="H4" s="194" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="I4" s="194" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="J4" s="190" t="s">
         <v>223</v>
@@ -4927,11 +4869,11 @@
       <c r="G5" s="190"/>
       <c r="H5" s="194" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="I5" s="194" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="J5" s="190" t="s">
         <v>227</v>
@@ -4959,11 +4901,11 @@
       <c r="G6" s="190"/>
       <c r="H6" s="194" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="I6" s="194" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="J6" s="190" t="s">
         <v>227</v>
@@ -5018,11 +4960,11 @@
       <c r="F11" s="190"/>
       <c r="G11" s="194" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="H11" s="194" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="I11" s="190" t="s">
         <v>223</v>
@@ -5048,11 +4990,11 @@
       <c r="F12" s="190"/>
       <c r="G12" s="194" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="H12" s="194" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="I12" s="190" t="s">
         <v>227</v>
@@ -5120,7 +5062,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.81"/>
@@ -5228,11 +5170,11 @@
       </c>
       <c r="E3" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387397</v>
+        <v>44720.6813204087</v>
       </c>
       <c r="F3" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387403</v>
+        <v>44720.6813204088</v>
       </c>
       <c r="G3" s="197"/>
       <c r="H3" s="197" t="s">
@@ -5267,14 +5209,14 @@
       </c>
       <c r="T3" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387411</v>
+        <v>44720.6813204089</v>
       </c>
       <c r="U3" s="199" t="s">
         <v>242</v>
       </c>
       <c r="V3" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387414</v>
+        <v>44720.681320409</v>
       </c>
       <c r="W3" s="197" t="s">
         <v>243</v>
@@ -5302,11 +5244,11 @@
       </c>
       <c r="E4" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387422</v>
+        <v>44720.6813204091</v>
       </c>
       <c r="F4" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387425</v>
+        <v>44720.6813204092</v>
       </c>
       <c r="G4" s="197"/>
       <c r="H4" s="197" t="s">
@@ -5341,14 +5283,14 @@
       </c>
       <c r="T4" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387433</v>
+        <v>44720.6813204093</v>
       </c>
       <c r="U4" s="199" t="s">
         <v>242</v>
       </c>
       <c r="V4" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387436</v>
+        <v>44720.6813204094</v>
       </c>
       <c r="W4" s="197" t="s">
         <v>243</v>
@@ -5376,11 +5318,11 @@
       </c>
       <c r="E5" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387444</v>
+        <v>44720.6813204095</v>
       </c>
       <c r="F5" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387446</v>
+        <v>44720.6813204096</v>
       </c>
       <c r="G5" s="197"/>
       <c r="H5" s="197" t="s">
@@ -5415,14 +5357,14 @@
       </c>
       <c r="T5" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387454</v>
+        <v>44720.6813204097</v>
       </c>
       <c r="U5" s="199" t="s">
         <v>242</v>
       </c>
       <c r="V5" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387457</v>
+        <v>44720.6813204097</v>
       </c>
       <c r="W5" s="197" t="s">
         <v>243</v>
@@ -5450,11 +5392,11 @@
       </c>
       <c r="E6" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387465</v>
+        <v>44720.6813204098</v>
       </c>
       <c r="F6" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387468</v>
+        <v>44720.6813204099</v>
       </c>
       <c r="G6" s="197"/>
       <c r="H6" s="197" t="s">
@@ -5489,14 +5431,14 @@
       </c>
       <c r="T6" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387475</v>
+        <v>44720.68132041</v>
       </c>
       <c r="U6" s="199" t="s">
         <v>242</v>
       </c>
       <c r="V6" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387478</v>
+        <v>44720.6813204101</v>
       </c>
       <c r="W6" s="197" t="s">
         <v>243</v>
@@ -5524,11 +5466,11 @@
       </c>
       <c r="E7" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387486</v>
+        <v>44720.6813204102</v>
       </c>
       <c r="F7" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387489</v>
+        <v>44720.6813204103</v>
       </c>
       <c r="G7" s="197"/>
       <c r="H7" s="197" t="s">
@@ -5563,14 +5505,14 @@
       </c>
       <c r="T7" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387496</v>
+        <v>44720.6813204104</v>
       </c>
       <c r="U7" s="199" t="s">
         <v>242</v>
       </c>
       <c r="V7" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387499</v>
+        <v>44720.6813204104</v>
       </c>
       <c r="W7" s="197" t="s">
         <v>243</v>
@@ -5598,11 +5540,11 @@
       </c>
       <c r="E8" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387508</v>
+        <v>44720.6813204105</v>
       </c>
       <c r="F8" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.676738751</v>
+        <v>44720.6813204106</v>
       </c>
       <c r="G8" s="197"/>
       <c r="H8" s="197" t="s">
@@ -5637,14 +5579,14 @@
       </c>
       <c r="T8" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387518</v>
+        <v>44720.6813204107</v>
       </c>
       <c r="U8" s="199" t="s">
         <v>242</v>
       </c>
       <c r="V8" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387523</v>
+        <v>44720.6813204108</v>
       </c>
       <c r="W8" s="197" t="s">
         <v>243</v>
@@ -5672,11 +5614,11 @@
       </c>
       <c r="E9" s="206" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387532</v>
+        <v>44720.6813204109</v>
       </c>
       <c r="F9" s="206" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387535</v>
+        <v>44720.6813204109</v>
       </c>
       <c r="G9" s="207"/>
       <c r="H9" s="207" t="s">
@@ -5711,14 +5653,14 @@
       </c>
       <c r="T9" s="206" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387543</v>
+        <v>44720.6813204111</v>
       </c>
       <c r="U9" s="199" t="s">
         <v>242</v>
       </c>
       <c r="V9" s="206" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387546</v>
+        <v>44720.6813204111</v>
       </c>
       <c r="W9" s="197" t="s">
         <v>243</v>
@@ -5746,11 +5688,11 @@
       </c>
       <c r="E10" s="206" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387552</v>
+        <v>44720.6813204112</v>
       </c>
       <c r="F10" s="206" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387556</v>
+        <v>44720.6813204113</v>
       </c>
       <c r="G10" s="207"/>
       <c r="H10" s="207" t="s">
@@ -5785,14 +5727,14 @@
       </c>
       <c r="T10" s="206" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387564</v>
+        <v>44720.6813204114</v>
       </c>
       <c r="U10" s="199" t="s">
         <v>242</v>
       </c>
       <c r="V10" s="206" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387567</v>
+        <v>44720.6813204115</v>
       </c>
       <c r="W10" s="197" t="s">
         <v>243</v>
@@ -5820,11 +5762,11 @@
       </c>
       <c r="E11" s="206" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387574</v>
+        <v>44720.6813204116</v>
       </c>
       <c r="F11" s="206" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387576</v>
+        <v>44720.6813204117</v>
       </c>
       <c r="G11" s="207"/>
       <c r="H11" s="207" t="s">
@@ -5859,14 +5801,14 @@
       </c>
       <c r="T11" s="206" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387585</v>
+        <v>44720.6813204118</v>
       </c>
       <c r="U11" s="199" t="s">
         <v>242</v>
       </c>
       <c r="V11" s="206" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387589</v>
+        <v>44720.6813204118</v>
       </c>
       <c r="W11" s="197" t="s">
         <v>243</v>
@@ -5894,11 +5836,11 @@
       </c>
       <c r="E12" s="206" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387595</v>
+        <v>44720.6813204119</v>
       </c>
       <c r="F12" s="206" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387598</v>
+        <v>44720.681320412</v>
       </c>
       <c r="G12" s="207"/>
       <c r="H12" s="207" t="s">
@@ -5933,14 +5875,14 @@
       </c>
       <c r="T12" s="206" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387607</v>
+        <v>44720.6813204121</v>
       </c>
       <c r="U12" s="199" t="s">
         <v>242</v>
       </c>
       <c r="V12" s="206" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.676738761</v>
+        <v>44720.6813204122</v>
       </c>
       <c r="W12" s="197" t="s">
         <v>243</v>
@@ -5968,11 +5910,11 @@
       </c>
       <c r="E13" s="206" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387617</v>
+        <v>44720.6813204123</v>
       </c>
       <c r="F13" s="206" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387619</v>
+        <v>44720.6813204124</v>
       </c>
       <c r="G13" s="207"/>
       <c r="H13" s="207" t="s">
@@ -6007,14 +5949,14 @@
       </c>
       <c r="T13" s="206" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387628</v>
+        <v>44720.6813204125</v>
       </c>
       <c r="U13" s="199" t="s">
         <v>242</v>
       </c>
       <c r="V13" s="206" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387632</v>
+        <v>44720.6813204125</v>
       </c>
       <c r="W13" s="197" t="s">
         <v>243</v>
@@ -6042,11 +5984,11 @@
       </c>
       <c r="E14" s="206" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387639</v>
+        <v>44720.6813204126</v>
       </c>
       <c r="F14" s="206" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387641</v>
+        <v>44720.6813204127</v>
       </c>
       <c r="G14" s="207"/>
       <c r="H14" s="207" t="s">
@@ -6081,14 +6023,14 @@
       </c>
       <c r="T14" s="206" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.676738765</v>
+        <v>44720.6813204128</v>
       </c>
       <c r="U14" s="199" t="s">
         <v>242</v>
       </c>
       <c r="V14" s="206" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387653</v>
+        <v>44720.6813204129</v>
       </c>
       <c r="W14" s="197" t="s">
         <v>243</v>
@@ -6116,11 +6058,11 @@
       </c>
       <c r="E15" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.676738766</v>
+        <v>44720.681320413</v>
       </c>
       <c r="F15" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387664</v>
+        <v>44720.681320413</v>
       </c>
       <c r="G15" s="197"/>
       <c r="H15" s="197" t="s">
@@ -6155,14 +6097,14 @@
       </c>
       <c r="T15" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387672</v>
+        <v>44720.6813204132</v>
       </c>
       <c r="U15" s="199" t="s">
         <v>242</v>
       </c>
       <c r="V15" s="200" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767387676</v>
+        <v>44720.6813204132</v>
       </c>
       <c r="W15" s="197" t="s">
         <v>243</v>
@@ -6199,7 +6141,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.22"/>
@@ -6268,11 +6210,11 @@
       </c>
       <c r="E3" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389002</v>
+        <v>44720.6813204456</v>
       </c>
       <c r="F3" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389005</v>
+        <v>44720.6813204457</v>
       </c>
       <c r="G3" s="208"/>
       <c r="H3" s="208" t="s">
@@ -6280,7 +6222,7 @@
       </c>
       <c r="I3" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767389009#1</v>
+        <v>c#44720.6813204458#1</v>
       </c>
     </row>
     <row r="4" s="177" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6298,11 +6240,11 @@
       </c>
       <c r="E4" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389015</v>
+        <v>44720.6813204465</v>
       </c>
       <c r="F4" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389018</v>
+        <v>44720.6813204466</v>
       </c>
       <c r="G4" s="208"/>
       <c r="H4" s="208" t="s">
@@ -6310,7 +6252,7 @@
       </c>
       <c r="I4" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767389021#1</v>
+        <v>c#44720.6813204467#1</v>
       </c>
     </row>
     <row r="5" s="177" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6328,11 +6270,11 @@
       </c>
       <c r="E5" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389027</v>
+        <v>44720.6813204469</v>
       </c>
       <c r="F5" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.676738903</v>
+        <v>44720.681320447</v>
       </c>
       <c r="G5" s="208"/>
       <c r="H5" s="208" t="s">
@@ -6340,7 +6282,7 @@
       </c>
       <c r="I5" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767389033#1</v>
+        <v>c#44720.6813204471#1</v>
       </c>
     </row>
     <row r="6" s="177" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6358,11 +6300,11 @@
       </c>
       <c r="E6" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389038</v>
+        <v>44720.6813204473</v>
       </c>
       <c r="F6" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.676738904</v>
+        <v>44720.6813204474</v>
       </c>
       <c r="G6" s="208"/>
       <c r="H6" s="208" t="s">
@@ -6370,7 +6312,7 @@
       </c>
       <c r="I6" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767389044#1</v>
+        <v>c#44720.6813204475#1</v>
       </c>
     </row>
     <row r="7" s="177" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6388,11 +6330,11 @@
       </c>
       <c r="E7" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389048</v>
+        <v>44720.6813204477</v>
       </c>
       <c r="F7" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389052</v>
+        <v>44720.6813204478</v>
       </c>
       <c r="G7" s="208"/>
       <c r="H7" s="208" t="s">
@@ -6400,7 +6342,7 @@
       </c>
       <c r="I7" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767389055#1</v>
+        <v>c#44720.6813204478#1</v>
       </c>
     </row>
     <row r="8" s="177" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6418,11 +6360,11 @@
       </c>
       <c r="E8" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.676738906</v>
+        <v>44720.6813204481</v>
       </c>
       <c r="F8" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389062</v>
+        <v>44720.6813204481</v>
       </c>
       <c r="G8" s="208"/>
       <c r="H8" s="208" t="s">
@@ -6430,7 +6372,7 @@
       </c>
       <c r="I8" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767389066#1</v>
+        <v>c#44720.6813204482#1</v>
       </c>
     </row>
     <row r="9" s="177" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6448,11 +6390,11 @@
       </c>
       <c r="E9" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.676738907</v>
+        <v>44720.6813204486</v>
       </c>
       <c r="F9" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389073</v>
+        <v>44720.6813204488</v>
       </c>
       <c r="G9" s="208"/>
       <c r="H9" s="208" t="s">
@@ -6460,7 +6402,7 @@
       </c>
       <c r="I9" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767389076#1</v>
+        <v>c#44720.6813204489#1</v>
       </c>
     </row>
     <row r="10" s="177" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6478,11 +6420,11 @@
       </c>
       <c r="E10" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389082</v>
+        <v>44720.6813204491</v>
       </c>
       <c r="F10" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389086</v>
+        <v>44720.6813204492</v>
       </c>
       <c r="G10" s="208"/>
       <c r="H10" s="208" t="s">
@@ -6490,7 +6432,7 @@
       </c>
       <c r="I10" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.676738909#1</v>
+        <v>c#44720.6813204492#1</v>
       </c>
     </row>
     <row r="11" s="177" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6508,11 +6450,11 @@
       </c>
       <c r="E11" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389095</v>
+        <v>44720.6813204495</v>
       </c>
       <c r="F11" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389097</v>
+        <v>44720.6813204496</v>
       </c>
       <c r="G11" s="208"/>
       <c r="H11" s="208" t="s">
@@ -6520,7 +6462,7 @@
       </c>
       <c r="I11" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.67673891#1</v>
+        <v>c#44720.6813204496#1</v>
       </c>
     </row>
     <row r="12" s="177" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6538,11 +6480,11 @@
       </c>
       <c r="E12" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389105</v>
+        <v>44720.6813204499</v>
       </c>
       <c r="F12" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389107</v>
+        <v>44720.6813204499</v>
       </c>
       <c r="G12" s="208"/>
       <c r="H12" s="208" t="s">
@@ -6550,7 +6492,7 @@
       </c>
       <c r="I12" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767389112#1</v>
+        <v>c#44720.68132045#1</v>
       </c>
     </row>
     <row r="13" s="177" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6568,11 +6510,11 @@
       </c>
       <c r="E13" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389117</v>
+        <v>44720.6813204503</v>
       </c>
       <c r="F13" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.676738912</v>
+        <v>44720.6813204503</v>
       </c>
       <c r="G13" s="208"/>
       <c r="H13" s="208" t="s">
@@ -6580,7 +6522,7 @@
       </c>
       <c r="I13" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767389123#1</v>
+        <v>c#44720.6813204504#1</v>
       </c>
     </row>
     <row r="14" s="177" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6598,11 +6540,11 @@
       </c>
       <c r="E14" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389127</v>
+        <v>44720.6813204506</v>
       </c>
       <c r="F14" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.676738913</v>
+        <v>44720.6813204507</v>
       </c>
       <c r="G14" s="208"/>
       <c r="H14" s="208" t="s">
@@ -6610,7 +6552,7 @@
       </c>
       <c r="I14" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767389133#1</v>
+        <v>c#44720.6813204508#1</v>
       </c>
     </row>
     <row r="15" s="177" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6628,11 +6570,11 @@
       </c>
       <c r="E15" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389139</v>
+        <v>44720.681320451</v>
       </c>
       <c r="F15" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389142</v>
+        <v>44720.6813204511</v>
       </c>
       <c r="G15" s="208"/>
       <c r="H15" s="208" t="s">
@@ -6640,7 +6582,7 @@
       </c>
       <c r="I15" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767389145#1</v>
+        <v>c#44720.6813204511#1</v>
       </c>
     </row>
     <row r="16" s="177" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6658,11 +6600,11 @@
       </c>
       <c r="E16" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389149</v>
+        <v>44720.6813204514</v>
       </c>
       <c r="F16" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389152</v>
+        <v>44720.6813204514</v>
       </c>
       <c r="G16" s="208"/>
       <c r="H16" s="208" t="s">
@@ -6670,7 +6612,7 @@
       </c>
       <c r="I16" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767389155#1</v>
+        <v>c#44720.6813204515#1</v>
       </c>
     </row>
     <row r="17" s="177" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6688,11 +6630,11 @@
       </c>
       <c r="E17" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.676738916</v>
+        <v>44720.6813204517</v>
       </c>
       <c r="F17" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389163</v>
+        <v>44720.6813204518</v>
       </c>
       <c r="G17" s="208"/>
       <c r="H17" s="208" t="s">
@@ -6700,7 +6642,7 @@
       </c>
       <c r="I17" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767389167#1</v>
+        <v>c#44720.6813204519#1</v>
       </c>
     </row>
     <row r="18" s="177" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6718,11 +6660,11 @@
       </c>
       <c r="E18" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389172</v>
+        <v>44720.6813204521</v>
       </c>
       <c r="F18" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389174</v>
+        <v>44720.6813204522</v>
       </c>
       <c r="G18" s="208"/>
       <c r="H18" s="208" t="s">
@@ -6730,7 +6672,7 @@
       </c>
       <c r="I18" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767389178#1</v>
+        <v>c#44720.6813204522#1</v>
       </c>
     </row>
     <row r="19" s="177" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6748,11 +6690,11 @@
       </c>
       <c r="E19" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389183</v>
+        <v>44720.6813204525</v>
       </c>
       <c r="F19" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389185</v>
+        <v>44720.6813204525</v>
       </c>
       <c r="G19" s="208"/>
       <c r="H19" s="208" t="s">
@@ -6760,7 +6702,7 @@
       </c>
       <c r="I19" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767389189#1</v>
+        <v>c#44720.6813204526#1</v>
       </c>
     </row>
     <row r="20" s="177" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6778,11 +6720,11 @@
       </c>
       <c r="E20" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389195</v>
+        <v>44720.6813204528</v>
       </c>
       <c r="F20" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389198</v>
+        <v>44720.6813204529</v>
       </c>
       <c r="G20" s="208"/>
       <c r="H20" s="208" t="s">
@@ -6790,7 +6732,7 @@
       </c>
       <c r="I20" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767389202#1</v>
+        <v>c#44720.681320453#1</v>
       </c>
     </row>
     <row r="21" s="177" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6808,11 +6750,11 @@
       </c>
       <c r="E21" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389206</v>
+        <v>44720.6813204533</v>
       </c>
       <c r="F21" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389209</v>
+        <v>44720.6813204533</v>
       </c>
       <c r="G21" s="208"/>
       <c r="H21" s="208" t="s">
@@ -6820,7 +6762,7 @@
       </c>
       <c r="I21" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767389212#1</v>
+        <v>c#44720.6813204534#1</v>
       </c>
     </row>
     <row r="22" s="177" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6838,11 +6780,11 @@
       </c>
       <c r="E22" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389217</v>
+        <v>44720.6813204536</v>
       </c>
       <c r="F22" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389219</v>
+        <v>44720.6813204537</v>
       </c>
       <c r="G22" s="208"/>
       <c r="H22" s="208" t="s">
@@ -6850,7 +6792,7 @@
       </c>
       <c r="I22" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767389224#1</v>
+        <v>c#44720.6813204538#1</v>
       </c>
     </row>
     <row r="23" s="177" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6868,11 +6810,11 @@
       </c>
       <c r="E23" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389229</v>
+        <v>44720.681320454</v>
       </c>
       <c r="F23" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389231</v>
+        <v>44720.6813204541</v>
       </c>
       <c r="G23" s="208"/>
       <c r="H23" s="208" t="s">
@@ -6880,7 +6822,7 @@
       </c>
       <c r="I23" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767389235#1</v>
+        <v>c#44720.6813204542#1</v>
       </c>
     </row>
     <row r="24" s="177" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6898,11 +6840,11 @@
       </c>
       <c r="E24" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389239</v>
+        <v>44720.6813204544</v>
       </c>
       <c r="F24" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389242</v>
+        <v>44720.6813204545</v>
       </c>
       <c r="G24" s="208"/>
       <c r="H24" s="208" t="s">
@@ -6910,7 +6852,7 @@
       </c>
       <c r="I24" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767389245#1</v>
+        <v>c#44720.6813204546#1</v>
       </c>
     </row>
     <row r="25" s="177" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6928,11 +6870,11 @@
       </c>
       <c r="E25" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389251</v>
+        <v>44720.6813204548</v>
       </c>
       <c r="F25" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389254</v>
+        <v>44720.6813204549</v>
       </c>
       <c r="G25" s="208"/>
       <c r="H25" s="208" t="s">
@@ -6940,7 +6882,7 @@
       </c>
       <c r="I25" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767389257#1</v>
+        <v>c#44720.681320455#1</v>
       </c>
     </row>
     <row r="26" s="177" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6958,11 +6900,11 @@
       </c>
       <c r="E26" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389261</v>
+        <v>44720.6813204552</v>
       </c>
       <c r="F26" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389264</v>
+        <v>44720.6813204553</v>
       </c>
       <c r="G26" s="208"/>
       <c r="H26" s="208" t="s">
@@ -6970,7 +6912,7 @@
       </c>
       <c r="I26" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767389267#1</v>
+        <v>c#44720.6813204553#1</v>
       </c>
     </row>
     <row r="27" s="177" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6988,11 +6930,11 @@
       </c>
       <c r="E27" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389272</v>
+        <v>44720.6813204556</v>
       </c>
       <c r="F27" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767389274</v>
+        <v>44720.6813204557</v>
       </c>
       <c r="G27" s="208"/>
       <c r="H27" s="208" t="s">
@@ -7000,7 +6942,7 @@
       </c>
       <c r="I27" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767389279#1</v>
+        <v>c#44720.6813204557#1</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7031,7 +6973,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.96"/>
@@ -7126,11 +7068,11 @@
       </c>
       <c r="G3" s="212" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767390599</v>
+        <v>44720.6813204902</v>
       </c>
       <c r="H3" s="212" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767390603</v>
+        <v>44720.6813204903</v>
       </c>
       <c r="I3" s="145"/>
       <c r="J3" s="145" t="s">
@@ -7138,7 +7080,7 @@
       </c>
       <c r="K3" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767390606#1</v>
+        <v>c#44720.6813204904#1</v>
       </c>
       <c r="L3" s="208" t="n">
         <v>0</v>
@@ -7165,11 +7107,11 @@
       </c>
       <c r="G4" s="212" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767390615</v>
+        <v>44720.6813204907</v>
       </c>
       <c r="H4" s="212" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767390618</v>
+        <v>44720.6813204908</v>
       </c>
       <c r="I4" s="145"/>
       <c r="J4" s="145" t="s">
@@ -7177,7 +7119,7 @@
       </c>
       <c r="K4" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767390623#1</v>
+        <v>c#44720.6813204909#1</v>
       </c>
       <c r="L4" s="208" t="n">
         <v>1</v>
@@ -7204,11 +7146,11 @@
       </c>
       <c r="G5" s="212" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767390629</v>
+        <v>44720.6813204911</v>
       </c>
       <c r="H5" s="212" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767390632</v>
+        <v>44720.6813204912</v>
       </c>
       <c r="I5" s="145"/>
       <c r="J5" s="145" t="s">
@@ -7216,7 +7158,7 @@
       </c>
       <c r="K5" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767390635#1</v>
+        <v>c#44720.6813204913#1</v>
       </c>
       <c r="L5" s="208" t="n">
         <v>2</v>
@@ -8512,7 +8454,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.65"/>
@@ -8598,11 +8540,11 @@
       </c>
       <c r="F3" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767393385</v>
+        <v>44720.6813205991</v>
       </c>
       <c r="G3" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.676739339</v>
+        <v>44720.6813205994</v>
       </c>
       <c r="H3" s="208"/>
       <c r="I3" s="208" t="s">
@@ -8610,7 +8552,7 @@
       </c>
       <c r="J3" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767393393#1</v>
+        <v>c#44720.6813205995#1</v>
       </c>
     </row>
     <row r="4" s="177" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8631,11 +8573,11 @@
       </c>
       <c r="F4" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767393399</v>
+        <v>44720.6813206</v>
       </c>
       <c r="G4" s="210" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767393401</v>
+        <v>44720.6813206001</v>
       </c>
       <c r="H4" s="208"/>
       <c r="I4" s="208" t="s">
@@ -8643,7 +8585,7 @@
       </c>
       <c r="J4" s="208" t="str">
         <f aca="true">_xlfn.CONCAT("c#",NOW(),"#1")</f>
-        <v>c#44717.6767393405#1</v>
+        <v>c#44720.6813206002#1</v>
       </c>
     </row>
   </sheetData>
@@ -12649,7 +12591,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.53"/>
@@ -17388,7 +17330,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.77"/>
@@ -17408,7 +17350,7 @@
       </c>
       <c r="B4" s="128" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17469,7 +17411,7 @@
       </c>
       <c r="B11" s="128" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17478,7 +17420,7 @@
       </c>
       <c r="B12" s="128" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17523,11 +17465,11 @@
   </sheetPr>
   <dimension ref="A1:Z48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O19" activeCellId="0" sqref="O19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T17" activeCellId="0" sqref="T17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="44.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.26"/>
@@ -17541,14 +17483,15 @@
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="10" min="10" style="0" width="13.12"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="11" min="11" style="0" width="17.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="21.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="10.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="20.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="14.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="35.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="9.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="8.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="15.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="8.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="32.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="10.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="12.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="9.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="0" width="18.52"/>
@@ -17641,7 +17584,7 @@
       </c>
       <c r="H2" s="142" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6756037089</v>
+        <v>44720.6813202362</v>
       </c>
       <c r="I2" s="141" t="n">
         <v>1</v>
@@ -17688,11 +17631,11 @@
       </c>
       <c r="X2" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382732</v>
+        <v>44720.6810500814</v>
       </c>
       <c r="Y2" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382737</v>
+        <v>44720.6810500823</v>
       </c>
       <c r="Z2" s="145"/>
     </row>
@@ -17711,7 +17654,7 @@
       </c>
       <c r="H3" s="142" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.675603709</v>
+        <v>44720.6813202382</v>
       </c>
       <c r="I3" s="141" t="n">
         <v>2</v>
@@ -17756,11 +17699,11 @@
       </c>
       <c r="X3" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382752</v>
+        <v>44720.6810500816</v>
       </c>
       <c r="Y3" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382754</v>
+        <v>44720.6810500824</v>
       </c>
       <c r="Z3" s="145"/>
     </row>
@@ -17779,7 +17722,7 @@
       </c>
       <c r="H4" s="142" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6756037091</v>
+        <v>44720.6813202386</v>
       </c>
       <c r="I4" s="141" t="n">
         <v>3</v>
@@ -17822,11 +17765,11 @@
       </c>
       <c r="X4" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382767</v>
+        <v>44720.6810500816</v>
       </c>
       <c r="Y4" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382769</v>
+        <v>44720.6810500824</v>
       </c>
       <c r="Z4" s="145"/>
     </row>
@@ -17845,7 +17788,7 @@
       </c>
       <c r="H5" s="142" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6756037091</v>
+        <v>44720.6813202389</v>
       </c>
       <c r="I5" s="141" t="n">
         <v>4</v>
@@ -17888,11 +17831,11 @@
       </c>
       <c r="X5" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382783</v>
+        <v>44720.6810500817</v>
       </c>
       <c r="Y5" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382786</v>
+        <v>44720.6810500824</v>
       </c>
       <c r="Z5" s="145"/>
     </row>
@@ -17909,7 +17852,7 @@
       </c>
       <c r="H6" s="142" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6756037091</v>
+        <v>44720.6813202391</v>
       </c>
       <c r="I6" s="141" t="n">
         <v>5</v>
@@ -17952,11 +17895,11 @@
       </c>
       <c r="X6" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382799</v>
+        <v>44720.6810500817</v>
       </c>
       <c r="Y6" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382802</v>
+        <v>44720.6810500825</v>
       </c>
       <c r="Z6" s="145"/>
     </row>
@@ -17975,7 +17918,7 @@
       </c>
       <c r="H7" s="142" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6756037092</v>
+        <v>44720.6813202395</v>
       </c>
       <c r="I7" s="141" t="n">
         <v>6</v>
@@ -18018,11 +17961,11 @@
       </c>
       <c r="X7" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382816</v>
+        <v>44720.6810500817</v>
       </c>
       <c r="Y7" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382818</v>
+        <v>44720.6810500825</v>
       </c>
       <c r="Z7" s="145"/>
     </row>
@@ -18041,7 +17984,7 @@
       </c>
       <c r="H8" s="142" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6756037092</v>
+        <v>44720.6813202403</v>
       </c>
       <c r="I8" s="141" t="n">
         <v>7</v>
@@ -18084,11 +18027,11 @@
       </c>
       <c r="X8" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.676738283</v>
+        <v>44720.6810500818</v>
       </c>
       <c r="Y8" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382833</v>
+        <v>44720.6810500825</v>
       </c>
       <c r="Z8" s="145" t="n">
         <v>9</v>
@@ -18107,7 +18050,7 @@
       </c>
       <c r="H9" s="142" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6756037092</v>
+        <v>44720.6813202406</v>
       </c>
       <c r="I9" s="141" t="n">
         <v>7</v>
@@ -18150,11 +18093,11 @@
       </c>
       <c r="X9" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382847</v>
+        <v>44720.6810500818</v>
       </c>
       <c r="Y9" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382849</v>
+        <v>44720.6810500825</v>
       </c>
       <c r="Z9" s="145" t="n">
         <v>8</v>
@@ -18175,7 +18118,7 @@
       </c>
       <c r="H10" s="142" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6756037092</v>
+        <v>44720.6813202408</v>
       </c>
       <c r="I10" s="141" t="n">
         <v>8</v>
@@ -18218,11 +18161,11 @@
       </c>
       <c r="X10" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382863</v>
+        <v>44720.6810500818</v>
       </c>
       <c r="Y10" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382866</v>
+        <v>44720.6810500826</v>
       </c>
       <c r="Z10" s="145"/>
     </row>
@@ -18241,7 +18184,7 @@
       </c>
       <c r="H11" s="142" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6756037093</v>
+        <v>44720.6813202411</v>
       </c>
       <c r="I11" s="141" t="n">
         <v>9</v>
@@ -18286,11 +18229,11 @@
       </c>
       <c r="X11" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.676738288</v>
+        <v>44720.6810500819</v>
       </c>
       <c r="Y11" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382883</v>
+        <v>44720.6810500826</v>
       </c>
       <c r="Z11" s="145" t="n">
         <v>11</v>
@@ -18307,7 +18250,7 @@
       </c>
       <c r="H12" s="142" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6756037093</v>
+        <v>44720.6813202414</v>
       </c>
       <c r="I12" s="141" t="n">
         <v>9</v>
@@ -18352,17 +18295,17 @@
       </c>
       <c r="X12" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.67673829</v>
+        <v>44720.6810500819</v>
       </c>
       <c r="Y12" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382903</v>
+        <v>44720.6810500826</v>
       </c>
       <c r="Z12" s="145" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="135.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="70.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="138" t="s">
         <v>154</v>
       </c>
@@ -18377,7 +18320,7 @@
       </c>
       <c r="H13" s="147" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6756037093</v>
+        <v>44720.6813202416</v>
       </c>
       <c r="I13" s="146" t="n">
         <v>9</v>
@@ -18422,11 +18365,11 @@
       </c>
       <c r="X13" s="149" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382917</v>
+        <v>44720.6810500819</v>
       </c>
       <c r="Y13" s="149" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382919</v>
+        <v>44720.6810500826</v>
       </c>
       <c r="Z13" s="150"/>
     </row>
@@ -18445,7 +18388,7 @@
       </c>
       <c r="H14" s="142" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6756037093</v>
+        <v>44720.6810746305</v>
       </c>
       <c r="M14" s="141"/>
       <c r="N14" s="141"/>
@@ -18462,11 +18405,11 @@
       <c r="W14" s="143"/>
       <c r="X14" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382929</v>
+        <v>44720.681050082</v>
       </c>
       <c r="Y14" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382931</v>
+        <v>44720.6810500827</v>
       </c>
       <c r="Z14" s="145"/>
     </row>
@@ -18476,7 +18419,7 @@
       </c>
       <c r="H15" s="142" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6756037094</v>
+        <v>44720.6810746325</v>
       </c>
       <c r="I15" s="141"/>
       <c r="J15" s="141"/>
@@ -18497,11 +18440,11 @@
       <c r="W15" s="143"/>
       <c r="X15" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382938</v>
+        <v>44720.681050082</v>
       </c>
       <c r="Y15" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.676738294</v>
+        <v>44720.6810500827</v>
       </c>
       <c r="Z15" s="145"/>
     </row>
@@ -18511,7 +18454,7 @@
       </c>
       <c r="H16" s="142" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6756037094</v>
+        <v>44720.6810746341</v>
       </c>
       <c r="I16" s="141"/>
       <c r="J16" s="141"/>
@@ -18532,11 +18475,11 @@
       <c r="W16" s="143"/>
       <c r="X16" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382947</v>
+        <v>44720.681050082</v>
       </c>
       <c r="Y16" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.676738295</v>
+        <v>44720.6810500827</v>
       </c>
       <c r="Z16" s="145"/>
     </row>
@@ -18555,7 +18498,7 @@
       </c>
       <c r="H17" s="142" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6756037094</v>
+        <v>44720.6810746357</v>
       </c>
       <c r="I17" s="141"/>
       <c r="J17" s="141"/>
@@ -18576,11 +18519,11 @@
       <c r="W17" s="143"/>
       <c r="X17" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382958</v>
+        <v>44720.6810500821</v>
       </c>
       <c r="Y17" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.676738296</v>
+        <v>44720.6810500827</v>
       </c>
       <c r="Z17" s="145"/>
     </row>
@@ -18600,7 +18543,7 @@
       </c>
       <c r="H18" s="142" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6756037094</v>
+        <v>44720.6810746376</v>
       </c>
       <c r="I18" s="141"/>
       <c r="J18" s="141"/>
@@ -18621,11 +18564,11 @@
       <c r="W18" s="143"/>
       <c r="X18" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382968</v>
+        <v>44720.6810500821</v>
       </c>
       <c r="Y18" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.676738297</v>
+        <v>44720.6810500828</v>
       </c>
       <c r="Z18" s="145"/>
     </row>
@@ -18645,7 +18588,7 @@
       </c>
       <c r="H19" s="142" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6756037095</v>
+        <v>44720.681074639</v>
       </c>
       <c r="I19" s="141"/>
       <c r="J19" s="141"/>
@@ -18666,11 +18609,11 @@
       <c r="W19" s="143"/>
       <c r="X19" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382979</v>
+        <v>44720.6810500821</v>
       </c>
       <c r="Y19" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382981</v>
+        <v>44720.6810500828</v>
       </c>
       <c r="Z19" s="145"/>
     </row>
@@ -18690,7 +18633,7 @@
       </c>
       <c r="H20" s="142" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6756037095</v>
+        <v>44720.6810746405</v>
       </c>
       <c r="I20" s="141"/>
       <c r="J20" s="141"/>
@@ -18711,11 +18654,11 @@
       <c r="W20" s="143"/>
       <c r="X20" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382989</v>
+        <v>44720.6810500822</v>
       </c>
       <c r="Y20" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767382991</v>
+        <v>44720.6810500828</v>
       </c>
       <c r="Z20" s="145"/>
     </row>
@@ -18735,7 +18678,7 @@
       </c>
       <c r="H21" s="142" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6756037095</v>
+        <v>44720.6810746419</v>
       </c>
       <c r="I21" s="141"/>
       <c r="J21" s="141"/>
@@ -18756,11 +18699,11 @@
       <c r="W21" s="143"/>
       <c r="X21" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767383</v>
+        <v>44720.6810500822</v>
       </c>
       <c r="Y21" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767383002</v>
+        <v>44720.6810500828</v>
       </c>
       <c r="Z21" s="145"/>
     </row>
@@ -18780,7 +18723,7 @@
       </c>
       <c r="H22" s="142" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6756037095</v>
+        <v>44720.6810746433</v>
       </c>
       <c r="I22" s="141"/>
       <c r="J22" s="141"/>
@@ -18801,11 +18744,11 @@
       <c r="W22" s="143"/>
       <c r="X22" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.676738301</v>
+        <v>44720.6810500823</v>
       </c>
       <c r="Y22" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767383012</v>
+        <v>44720.6810500829</v>
       </c>
       <c r="Z22" s="145"/>
     </row>
@@ -18825,7 +18768,7 @@
       </c>
       <c r="H23" s="142" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6756037096</v>
+        <v>44720.6813202432</v>
       </c>
       <c r="I23" s="141" t="n">
         <v>10</v>
@@ -18850,11 +18793,11 @@
       <c r="W23" s="143"/>
       <c r="X23" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767383022</v>
+        <v>44720.6810500823</v>
       </c>
       <c r="Y23" s="144" t="n">
         <f aca="true">NOW()</f>
-        <v>44717.6767383025</v>
+        <v>44720.6810500829</v>
       </c>
       <c r="Z23" s="145"/>
     </row>
@@ -19071,7 +19014,7 @@
       <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.15"/>
@@ -19159,7 +19102,7 @@
       </c>
       <c r="B4" s="163" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="C4" s="127" t="n">
         <v>1</v>
@@ -19193,20 +19136,20 @@
       </c>
       <c r="M4" s="168" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="N4" s="168" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>44720</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="162" t="n">
         <v>2</v>
       </c>
       <c r="B5" s="163" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="C5" s="129" t="s">
         <v>194</v>
@@ -19240,11 +19183,11 @@
       </c>
       <c r="M5" s="168" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="N5" s="168" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19253,7 +19196,7 @@
       </c>
       <c r="B6" s="163" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="C6" s="129" t="s">
         <v>194</v>
@@ -19287,11 +19230,11 @@
       </c>
       <c r="M6" s="168" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="N6" s="168" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19300,7 +19243,7 @@
       </c>
       <c r="B7" s="163" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="C7" s="129" t="s">
         <v>194</v>
@@ -19334,11 +19277,11 @@
       </c>
       <c r="M7" s="168" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="N7" s="168" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19347,7 +19290,7 @@
       </c>
       <c r="B8" s="163" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="C8" s="127" t="n">
         <v>1</v>
@@ -19380,11 +19323,11 @@
       </c>
       <c r="M8" s="168" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="N8" s="168" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19393,7 +19336,7 @@
       </c>
       <c r="B9" s="163" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="C9" s="127" t="n">
         <v>1</v>
@@ -19426,11 +19369,11 @@
       </c>
       <c r="M9" s="168" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="N9" s="168" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19439,7 +19382,7 @@
       </c>
       <c r="B10" s="163" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="C10" s="127" t="n">
         <v>1</v>
@@ -19477,7 +19420,7 @@
       </c>
       <c r="B11" s="163" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="C11" s="127" t="n">
         <v>1</v>
@@ -19515,7 +19458,7 @@
       </c>
       <c r="B12" s="163" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="C12" s="127" t="n">
         <v>2</v>
@@ -19553,7 +19496,7 @@
       </c>
       <c r="B13" s="163" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="C13" s="127" t="n">
         <v>2</v>
@@ -19595,7 +19538,7 @@
       </c>
       <c r="B14" s="163" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="C14" s="127" t="n">
         <v>2</v>
@@ -19637,7 +19580,7 @@
       </c>
       <c r="B15" s="163" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="C15" s="127" t="n">
         <v>2</v>
@@ -19679,7 +19622,7 @@
       </c>
       <c r="B16" s="163" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="C16" s="127" t="n">
         <v>2</v>
@@ -19721,7 +19664,7 @@
       </c>
       <c r="B17" s="163" t="n">
         <f aca="true">TODAY()</f>
-        <v>44717</v>
+        <v>44720</v>
       </c>
       <c r="C17" s="127" t="n">
         <v>2</v>

</xml_diff>